<commit_message>
Made a more extensible version of level 3
</commit_message>
<xml_diff>
--- a/Sniper GOAT.xlsx
+++ b/Sniper GOAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80869AF-D96F-49C1-8D81-06FDE5CDEFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CD9F1CA-FC23-49F9-9674-22DBF20AB13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E63FEAF0-1E5E-4907-9FA7-7687370CAB07}"/>
   </bookViews>
@@ -2973,6 +2973,9 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2999,9 +3002,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3452,25 +3452,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="60.75" customHeight="1">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
     </row>
     <row r="3" spans="2:18" ht="15" customHeight="1">
       <c r="B3" s="1"/>
@@ -3483,67 +3483,67 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:18" ht="24" customHeight="1">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
     </row>
     <row r="5" spans="2:18" ht="48.75" customHeight="1">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="67" t="s">
         <v>593</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
     </row>
     <row r="6" spans="2:18" ht="25.5" customHeight="1">
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
     </row>
     <row r="7" spans="2:18" ht="15" customHeight="1">
       <c r="B7" s="4"/>
@@ -3605,16 +3605,16 @@
         <f>IF(ISBLANK(E11),0,IF(Answers!E11=E11,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="59" t="s">
         <v>590</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="61"/>
     </row>
     <row r="12" spans="2:18" ht="31.5" customHeight="1">
       <c r="B12" s="13" t="s">
@@ -3631,16 +3631,16 @@
         <f>IF(ISBLANK(E12),0,IF(Answers!E12=E12,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="59" t="s">
         <v>591</v>
       </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
     </row>
     <row r="13" spans="2:18" ht="42" customHeight="1">
       <c r="B13" s="18" t="s">
@@ -3657,16 +3657,16 @@
         <f>IF(ISBLANK(E13),0,IF(Answers!E13=E13,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="59" t="s">
         <v>592</v>
       </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="61"/>
     </row>
     <row r="14" spans="2:18" ht="31.5" customHeight="1">
       <c r="B14" s="13" t="s">
@@ -3683,16 +3683,16 @@
         <f>IF(ISBLANK(E14),0,IF(Answers!E14=E14,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="59" t="s">
         <v>589</v>
       </c>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
     </row>
     <row r="15" spans="2:18" ht="21" customHeight="1">
       <c r="B15" s="4"/>
@@ -3726,17 +3726,17 @@
       <c r="R16" s="5"/>
     </row>
     <row r="17" spans="2:11" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="I17" s="61" t="str" cm="1">
+      <c r="I17" s="62" t="str" cm="1">
         <f t="array" ref="I17">SUMPRODUCT(--(F:F&gt;0),D:D)&amp;"/"&amp;SUM(D:D)</f>
         <v>0/270</v>
       </c>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
     </row>
     <row r="18" spans="2:11" ht="15" thickBot="1">
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
     </row>
     <row r="19" spans="2:11" ht="24.75" customHeight="1" thickBot="1">
       <c r="B19" s="29" t="s">
@@ -3748,14 +3748,14 @@
       <c r="D19" s="23"/>
       <c r="E19" s="7"/>
       <c r="G19"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1">
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1">
       <c r="B21" s="6" t="s">
@@ -7535,8 +7535,8 @@
   </sheetPr>
   <dimension ref="A2:NUF484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView tabSelected="1" topLeftCell="E70" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R74" sqref="R74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.703125" defaultRowHeight="14.4"/>
@@ -7568,25 +7568,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:60" ht="60.75" customHeight="1">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
     </row>
     <row r="3" spans="2:60" ht="15" customHeight="1">
       <c r="B3" s="1"/>
@@ -7599,67 +7599,67 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:60" ht="24" customHeight="1">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="65" t="s">
         <v>660</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
     </row>
     <row r="5" spans="2:60" ht="48.75" customHeight="1">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="67" t="s">
         <v>663</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
     </row>
     <row r="6" spans="2:60" ht="25.5" customHeight="1">
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="65" t="s">
         <v>661</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
     </row>
     <row r="7" spans="2:60" ht="15" customHeight="1">
       <c r="B7" s="4"/>
@@ -7722,28 +7722,28 @@
         <f>IF(ISBLANK(E11),0,IF(Answers!E11=E11,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="59" t="s">
         <v>673</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="K11" s="59" t="s">
+      <c r="K11" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="L11" s="59" t="s">
+      <c r="L11" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="N11" s="60" t="s">
+      <c r="N11" s="61" t="s">
         <v>670</v>
       </c>
       <c r="AQ11" s="50" t="s">
@@ -7777,28 +7777,28 @@
         <f>IF(ISBLANK(E12),0,IF(Answers!E12=E12,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="59" t="s">
         <v>671</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="I12" s="59" t="s">
+      <c r="I12" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="K12" s="59" t="s">
+      <c r="K12" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="L12" s="59" t="s">
+      <c r="L12" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="M12" s="59" t="s">
+      <c r="M12" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="N12" s="60" t="s">
+      <c r="N12" s="61" t="s">
         <v>670</v>
       </c>
       <c r="AR12" s="2" t="str" cm="1">
@@ -7851,28 +7851,28 @@
         <f>IF(ISBLANK(E13),0,IF(Answers!E13=E13,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="59" t="s">
         <v>674</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="J13" s="59" t="s">
+      <c r="J13" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="K13" s="59" t="s">
+      <c r="K13" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="L13" s="59" t="s">
+      <c r="L13" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="M13" s="59" t="s">
+      <c r="M13" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="N13" s="60" t="s">
+      <c r="N13" s="61" t="s">
         <v>670</v>
       </c>
       <c r="AR13" s="2" t="str">
@@ -7925,28 +7925,28 @@
         <f>IF(ISBLANK(E14),0,IF(Answers!E14=E14,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="59" t="s">
         <v>672</v>
       </c>
-      <c r="H14" s="59" t="s">
+      <c r="H14" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="K14" s="59" t="s">
+      <c r="K14" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="M14" s="59" t="s">
+      <c r="M14" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="N14" s="60" t="s">
+      <c r="N14" s="61" t="s">
         <v>670</v>
       </c>
       <c r="AR14" s="2" t="str">
@@ -8072,12 +8072,12 @@
       </c>
     </row>
     <row r="17" spans="2:53" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="I17" s="61" t="str" cm="1">
+      <c r="I17" s="62" t="str" cm="1">
         <f t="array" ref="I17">SUMPRODUCT(--(F:F&gt;0),D:D)&amp;"/"&amp;SUM(D:D)</f>
         <v>90/270</v>
       </c>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2" t="str">
         <v>F6</v>
@@ -8111,9 +8111,9 @@
       </c>
     </row>
     <row r="18" spans="2:53" ht="15" thickBot="1">
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
       <c r="AR18" s="2" t="str">
         <v>I8</v>
       </c>
@@ -8155,9 +8155,9 @@
       <c r="D19" s="23"/>
       <c r="E19" s="7"/>
       <c r="G19"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
       <c r="AR19" s="2" t="str">
         <v>E4</v>
       </c>
@@ -8190,9 +8190,9 @@
       </c>
     </row>
     <row r="20" spans="2:53" ht="15" customHeight="1">
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
       <c r="AR20" s="2" t="str">
         <v>A2</v>
       </c>
@@ -51645,19 +51645,19 @@
         <v>102</v>
       </c>
       <c r="N74" s="42" t="e" cm="1">
-        <f t="array" aca="1" ref="N74" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.ANCHORARRAY(Q74),Q73:AMB73)))</f>
+        <f t="array" aca="1" ref="N74" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($Q$74:Q74)),_xlfn.ANCHORARRAY($Q$73))))</f>
         <v>#N/A</v>
       </c>
       <c r="O74" s="42" t="e" cm="1">
-        <f t="array" aca="1" ref="O74" ca="1">_xlfn.XMATCH(INDEX(_xlfn.ANCHORARRAY(Q74),,N74),_xlfn.ANCHORARRAY(Q73))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P74" s="42" t="b">
-        <f t="shared" ref="P74:P77" ca="1" si="3">_xlfn.IFNA(O74/10=N74-1,FALSE)</f>
+        <f t="array" aca="1" ref="O74" ca="1">_xlfn.XMATCH(INDEX(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($N$74:N74)),,N74),_xlfn.ANCHORARRAY($Q$73))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P74" s="42" t="b" cm="1">
+        <f t="array" aca="1" ref="P74:P78" ca="1">_xlfn.IFNA(O74:O78/10=N74:N78-1,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="Q74" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="Q74:AMB74" ca="1">ADDRESS(ROW(INDIRECT(INDEX(I73:I84, N72))), COLUMN(INDIRECT(INDEX(I73:I84, N72))) + _xlfn.SEQUENCE(1, 1000, 0, 1), 4)</f>
+      <c r="Q74" s="58" t="str" cm="1">
+        <f t="array" aca="1" ref="Q74:AMB78" ca="1">ADDRESS(ROW(INDIRECT(INDEX(I73:M84, $N$72,_xlfn.SEQUENCE(5)))), COLUMN(INDIRECT(INDEX(I73:M84, $N$72,_xlfn.SEQUENCE(5)))) + _xlfn.SEQUENCE(1, 1000, 0, 1), 4)</f>
         <v>WH8</v>
       </c>
       <c r="R74" s="42" t="str">
@@ -55696,19 +55696,19 @@
         <v>129</v>
       </c>
       <c r="N75" s="42" cm="1">
-        <f t="array" aca="1" ref="N75" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.ANCHORARRAY(Q75),Q73:AMB73)))</f>
+        <f t="array" aca="1" ref="N75" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($Q$74:Q75)),_xlfn.ANCHORARRAY($Q$73))))</f>
         <v>73</v>
       </c>
       <c r="O75" s="42" cm="1">
-        <f t="array" aca="1" ref="O75" ca="1">_xlfn.XMATCH(INDEX(_xlfn.ANCHORARRAY(Q75),,N75),_xlfn.ANCHORARRAY(Q73))</f>
+        <f t="array" aca="1" ref="O75" ca="1">_xlfn.XMATCH(INDEX(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($N$74:N75)),,N75),_xlfn.ANCHORARRAY($Q$73))</f>
         <v>720</v>
       </c>
       <c r="P75" s="42" t="b">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="Q75" s="48" t="str" cm="1">
-        <f t="array" aca="1" ref="Q75:AMB75" ca="1">ADDRESS(ROW(INDIRECT(INDEX(J73:J84, N72))), COLUMN(INDIRECT(INDEX(J73:J84, N72))) + _xlfn.SEQUENCE(1, 1000, 0, 1), 4)</f>
+      <c r="Q75" s="48" t="str">
+        <f ca="1"/>
         <v>DDA6481</v>
       </c>
       <c r="R75" s="42" t="str">
@@ -59747,19 +59747,19 @@
         <v>133</v>
       </c>
       <c r="N76" s="42" cm="1">
-        <f t="array" aca="1" ref="N76" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.ANCHORARRAY(Q76),Q73:AMB73)))</f>
+        <f t="array" aca="1" ref="N76" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($Q$74:Q76)),_xlfn.ANCHORARRAY($Q$73))))</f>
         <v>7</v>
       </c>
       <c r="O76" s="42" cm="1">
-        <f t="array" aca="1" ref="O76" ca="1">_xlfn.XMATCH(INDEX(_xlfn.ANCHORARRAY(Q76),,N76),_xlfn.ANCHORARRAY(Q73))</f>
+        <f t="array" aca="1" ref="O76" ca="1">_xlfn.XMATCH(INDEX(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($N$74:N76)),,N76),_xlfn.ANCHORARRAY($Q$73))</f>
         <v>60</v>
       </c>
       <c r="P76" s="42" t="b">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="Q76" s="48" t="str" cm="1">
-        <f t="array" aca="1" ref="Q76:AMB76" ca="1">ADDRESS(ROW(INDIRECT(INDEX(K73:K84, N72))), COLUMN(INDIRECT(INDEX(K73:K84, N72))) + _xlfn.SEQUENCE(1, 1000, 0, 1), 4)</f>
+      <c r="Q76" s="48" t="str">
+        <f ca="1"/>
         <v>IA541</v>
       </c>
       <c r="R76" s="42" t="str">
@@ -63798,19 +63798,19 @@
         <v>126</v>
       </c>
       <c r="N77" s="42" t="e" cm="1">
-        <f t="array" aca="1" ref="N77" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.ANCHORARRAY(Q77),Q73:AMB73)))</f>
+        <f t="array" aca="1" ref="N77" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($Q$74:Q77)),_xlfn.ANCHORARRAY($Q$73))))</f>
         <v>#N/A</v>
       </c>
       <c r="O77" s="42" t="e" cm="1">
-        <f t="array" aca="1" ref="O77" ca="1">_xlfn.XMATCH(INDEX(_xlfn.ANCHORARRAY(Q77),,N77),_xlfn.ANCHORARRAY(Q73))</f>
+        <f t="array" aca="1" ref="O77" ca="1">_xlfn.XMATCH(INDEX(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($N$74:N77)),,N77),_xlfn.ANCHORARRAY($Q$73))</f>
         <v>#N/A</v>
       </c>
       <c r="P77" s="42" t="b">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Q77" s="48" t="str" cm="1">
-        <f t="array" aca="1" ref="Q77:AMB77" ca="1">ADDRESS(ROW(INDIRECT(INDEX(L73:L84, N72))), COLUMN(INDIRECT(INDEX(L73:L84, N72))) + _xlfn.SEQUENCE(1, 1000, 0, 1), 4)</f>
+      <c r="Q77" s="48" t="str">
+        <f ca="1"/>
         <v>RJ9</v>
       </c>
       <c r="R77" s="42" t="str">
@@ -67849,19 +67849,19 @@
         <v>113</v>
       </c>
       <c r="N78" s="42" t="e" cm="1">
-        <f t="array" aca="1" ref="N78" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.ANCHORARRAY(Q78),Q73:AMB73)))</f>
+        <f t="array" aca="1" ref="N78" ca="1">_xlfn.XMATCH(TRUE,ISNUMBER(_xlfn.XMATCH(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($Q$74:Q78)),_xlfn.ANCHORARRAY($Q$73))))</f>
         <v>#N/A</v>
       </c>
       <c r="O78" s="42" t="e" cm="1">
-        <f t="array" aca="1" ref="O78" ca="1">_xlfn.XMATCH(INDEX(_xlfn.ANCHORARRAY(Q78),,N78),_xlfn.ANCHORARRAY(Q73))</f>
+        <f t="array" aca="1" ref="O78" ca="1">_xlfn.XMATCH(INDEX(_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY($Q$74),ROWS($N$74:N78)),,N78),_xlfn.ANCHORARRAY($Q$73))</f>
         <v>#N/A</v>
       </c>
       <c r="P78" s="42" t="b">
-        <f ca="1">_xlfn.IFNA(O78/10=N78-1,FALSE)</f>
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Q78" s="48" t="str" cm="1">
-        <f t="array" aca="1" ref="Q78:AMB78" ca="1">ADDRESS(ROW(INDIRECT(INDEX(M73:M84, N72))), COLUMN(INDIRECT(INDEX(M73:M84, N72))) + _xlfn.SEQUENCE(1, 1000, 0, 1), 4)</f>
+      <c r="Q78" s="48" t="str">
+        <f ca="1"/>
         <v>VC26</v>
       </c>
       <c r="R78" s="42" t="str">
@@ -72135,7 +72135,10 @@
       <c r="M84" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="N84" s="42"/>
+      <c r="N84" s="42" t="str" cm="1">
+        <f t="array" aca="1" ref="N84" ca="1">INDEX(Q75:AMB75,,720)</f>
+        <v>EER6481</v>
+      </c>
       <c r="P84" s="42"/>
       <c r="Q84" s="48">
         <v>6</v>
@@ -78924,25 +78927,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="60.75" customHeight="1">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>662</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
     </row>
     <row r="3" spans="2:18" ht="15" customHeight="1">
       <c r="B3" s="1"/>
@@ -78955,67 +78958,67 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:18" ht="24" customHeight="1">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
     </row>
     <row r="5" spans="2:18" ht="48.75" customHeight="1">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="67" t="s">
         <v>593</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
     </row>
     <row r="6" spans="2:18" ht="25.5" customHeight="1">
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
     </row>
     <row r="7" spans="2:18" ht="15" customHeight="1">
       <c r="B7" s="4"/>
@@ -79076,16 +79079,16 @@
         <v>3</v>
       </c>
       <c r="F11" s="25"/>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="59" t="s">
         <v>590</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="61"/>
     </row>
     <row r="12" spans="2:18" ht="31.5" customHeight="1">
       <c r="B12" s="13" t="s">
@@ -79101,16 +79104,16 @@
         <v>159</v>
       </c>
       <c r="F12" s="25"/>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="59" t="s">
         <v>591</v>
       </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
     </row>
     <row r="13" spans="2:18" ht="42" customHeight="1">
       <c r="B13" s="18" t="s">
@@ -79126,16 +79129,16 @@
         <v>145</v>
       </c>
       <c r="F13" s="25"/>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="59" t="s">
         <v>592</v>
       </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="61"/>
     </row>
     <row r="14" spans="2:18" ht="31.5" customHeight="1">
       <c r="B14" s="13" t="s">
@@ -79151,16 +79154,16 @@
         <v>-532.857736549165</v>
       </c>
       <c r="F14" s="25"/>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="59" t="s">
         <v>589</v>
       </c>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
     </row>
     <row r="15" spans="2:18" ht="21" customHeight="1">
       <c r="B15" s="4"/>
@@ -79194,14 +79197,14 @@
       <c r="R16" s="5"/>
     </row>
     <row r="17" spans="2:11" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
     </row>
     <row r="18" spans="2:11" ht="15" thickBot="1">
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
     </row>
     <row r="19" spans="2:11" ht="24.75" customHeight="1" thickBot="1">
       <c r="B19" s="29" t="s">
@@ -79213,14 +79216,14 @@
       <c r="D19" s="23"/>
       <c r="E19" s="7"/>
       <c r="G19"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1">
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1">
       <c r="B21" s="6" t="s">

</xml_diff>